<commit_message>
Modify directory and file name
</commit_message>
<xml_diff>
--- a/output/OPEN/MOESCHETQ22001535/MOESCHETQ22001535.xlsx
+++ b/output/OPEN/MOESCHETQ22001535/MOESCHETQ22001535.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project1\output\OPEN\MOESCHETQ22001535\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6431dddeb4959f/Documents/UiPath/Diamond/Project1/output/OPEN/MOESCHETQ22001535/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_3200EB49F9B987C1BE8A34A726EF624E62EEE57C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B537AAB7-19C2-41AA-AFF9-709E62ACED19}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="8340"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,14 +411,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.6328125" customWidth="1"/>
+    <col min="2" max="2" width="75.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -433,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -441,7 +448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -449,7 +456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -457,7 +464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -465,7 +472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -473,7 +480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -481,7 +488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -489,7 +496,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -497,7 +504,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -505,7 +512,7 @@
         <v>67676750</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -513,7 +520,7 @@
         <v>67676751</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -527,12 +534,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>